<commit_message>
added jul event (#1003)
Co-authored-by: way0utwest <admin@sqlsaturday.com>
</commit_message>
<xml_diff>
--- a/assets/misc/2025/2025_Attendance.xlsx
+++ b/assets/misc/2025/2025_Attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47D2F1A-6C43-44B4-8472-576BEAA6B372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5C2815-CB05-4CD7-8ACB-5B0A5D633825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25545" yWindow="1260" windowWidth="21765" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20940" yWindow="1425" windowWidth="17970" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Event</t>
   </si>
@@ -75,6 +75,39 @@
   </si>
   <si>
     <t>SQL Saturday Richmond 2025 (#1106)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Austin 2025 (#1112)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Orange County 2025 (#1115)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Jacksonville 2025 (#1103)</t>
+  </si>
+  <si>
+    <t>SeaQL Saturday 2025 (#1101)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Haiti 2025 (#1109) - Virtual</t>
+  </si>
+  <si>
+    <t>SQL Saturday New York City 2025 (#1105)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Raleigh 2025 (#1111)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Salt Lake City 2025 (#1114)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Trujillo 2025 (#1118)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Montreal 2025 (#1121)</t>
+  </si>
+  <si>
+    <t>SQL Saturday San Diego 2025 (#1113)</t>
   </si>
 </sst>
 </file>
@@ -141,13 +174,10 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -441,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,10 +516,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>45724</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2">
@@ -504,10 +534,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>45738</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C3">
@@ -522,10 +552,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>45752</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C4">
@@ -540,152 +570,284 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>45752</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="C5">
+        <v>162</v>
+      </c>
+      <c r="D5">
+        <v>98</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E17" si="0">IF(C5=0,0,+(C5-D5)/C5)</f>
+        <v>0.39506172839506171</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="4">
+        <v>45773</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>121</v>
+      </c>
+      <c r="D6">
+        <v>400</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.3057851239669422</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="4">
+        <v>45759</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="4">
+        <v>45780</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>122</v>
+      </c>
+      <c r="D8">
+        <v>74</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.39344262295081966</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="4">
+        <v>45780</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="4">
+        <v>45780</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>578</v>
+      </c>
+      <c r="D10">
+        <v>499</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.13667820069204153</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="4">
+        <v>45787</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="4">
+        <v>45794</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="4">
+        <v>45800</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="4">
+        <v>45822</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="4">
+        <v>45822</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="4"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="4">
+        <v>45836</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="4"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="4"/>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="4"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="4"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="A23" s="4"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+      <c r="A24" s="4"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+      <c r="A25" s="4"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="A26" s="4"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="4"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="7"/>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="6"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="6"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="7"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="6"/>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="6"/>
       <c r="E33" s="1"/>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="6"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="7"/>
+      <c r="E35" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I14">
-    <sortCondition ref="A2:A14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://sqlsaturday.com/2025-03-08-sqlsaturday1102/" xr:uid="{DB7DCC26-7A8C-496A-AA86-D6D85137F569}"/>
     <hyperlink ref="B3" r:id="rId2" display="https://sqlsaturday.com/2025-03-22-sqlsaturday1108/" xr:uid="{EB68852C-9679-4DE9-8BDC-C57E12F98B82}"/>
     <hyperlink ref="B4" r:id="rId3" display="https://sqlsaturday.com/2025-04-05-sqlsaturday1104/" xr:uid="{07498ECC-2342-4161-A4D2-9664C3E2305E}"/>
     <hyperlink ref="B5" r:id="rId4" display="https://sqlsaturday.com/2025-04-05-sqlsaturday1106/" xr:uid="{A0AC7D18-AEAB-4F12-90B5-8E9B77797994}"/>
+    <hyperlink ref="B8" r:id="rId5" display="https://sqlsaturday.com/2025-05-03-sqlsaturday1112/" xr:uid="{407391C8-D47F-4A8B-8DEA-63C69D0D44A0}"/>
+    <hyperlink ref="B9" r:id="rId6" display="https://sqlsaturday.com/2025-05-03-sqlsaturday1115" xr:uid="{81D03EC4-EF29-431A-B5B5-D6DC6337E9A0}"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://sqlsaturday.com/2025-05-03-sqlsaturday1103/" xr:uid="{B3E1E047-321A-4438-B3CB-D2CDF0624593}"/>
+    <hyperlink ref="B7" r:id="rId8" display="https://sqlsaturday.com/2025-04-12-sqlsaturday1101/" xr:uid="{3DE3CBCE-62FF-4222-BEC2-58BE68B24EA7}"/>
+    <hyperlink ref="B6" r:id="rId9" display="https://sqlsaturday.com/2025-04-26-sqlsaturday1109/" xr:uid="{DDC0B63E-3C7C-4AEB-934A-F03AEC067F39}"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://sqlsaturday.com/2025-05-10-sqlsaturday1105/" xr:uid="{DE358FDC-D191-4EEE-BA27-A0B7A81F1F0A}"/>
+    <hyperlink ref="B12" r:id="rId11" display="https://sqlsaturday.com/2025-05-17-sqlsaturday1111/" xr:uid="{C9F54A79-C8AE-4FB0-AAAC-825EF00BED8B}"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://sqlsaturday.com/2025-05-23-sqlsaturday1114/" xr:uid="{E626B63A-9A1B-4203-A598-5262C955BEE3}"/>
+    <hyperlink ref="B14" r:id="rId13" display="https://sqlsaturday.com/2025-06-14-sqlsaturday1118/" xr:uid="{79456440-FBCF-4572-9A31-E79BA788EEA0}"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://sqlsaturday.com/2025-06-14-sqlsaturday1121/" xr:uid="{C9CD811F-8607-42B7-8E8D-1E211A855697}"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://sqlsaturday.com/2025-06-28-sqlsaturday1113/" xr:uid="{E09BC4EF-E940-4CAC-A994-2F854354F7F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
slc update from organizer
</commit_message>
<xml_diff>
--- a/assets/misc/2025/2025_Attendance.xlsx
+++ b/assets/misc/2025/2025_Attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve.jones\Documents\git\sqlsatwebsite\assets\misc\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D83353-E3F5-408E-AB47-0EFF52EF5E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCBCF11-12C8-4A23-8228-03C4011C2959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30855" yWindow="75" windowWidth="21840" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,20 +473,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -515,7 +515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45724</v>
       </c>
@@ -533,7 +533,7 @@
         <v>0.3953033268101761</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>45738</v>
       </c>
@@ -551,7 +551,7 @@
         <v>0.47619047619047616</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>45752</v>
       </c>
@@ -569,7 +569,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>45752</v>
       </c>
@@ -587,7 +587,7 @@
         <v>0.39506172839506171</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>45773</v>
       </c>
@@ -605,7 +605,7 @@
         <v>-2.3057851239669422</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>45759</v>
       </c>
@@ -623,7 +623,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>45780</v>
       </c>
@@ -641,7 +641,7 @@
         <v>0.31147540983606559</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>45780</v>
       </c>
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>45780</v>
       </c>
@@ -671,7 +671,7 @@
         <v>0.13667820069204153</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>45787</v>
       </c>
@@ -689,7 +689,7 @@
         <v>0.11627906976744186</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>45794</v>
       </c>
@@ -707,19 +707,25 @@
         <v>0.34444444444444444</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>45800</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="C13">
+        <v>171</v>
+      </c>
+      <c r="D13">
+        <v>80</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.53216374269005851</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>45822</v>
       </c>
@@ -731,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>45822</v>
       </c>
@@ -743,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>45836</v>
       </c>
@@ -755,91 +761,91 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="6"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="6"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="6"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="6"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="B34" s="6"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
       <c r="B35" s="7"/>
       <c r="E35" s="1"/>

</xml_diff>

<commit_message>
slc update from organizer (#1046)
</commit_message>
<xml_diff>
--- a/assets/misc/2025/2025_Attendance.xlsx
+++ b/assets/misc/2025/2025_Attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve.jones\Documents\git\sqlsatwebsite\assets\misc\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D83353-E3F5-408E-AB47-0EFF52EF5E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCBCF11-12C8-4A23-8228-03C4011C2959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30855" yWindow="75" windowWidth="21840" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,20 +473,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -515,7 +515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45724</v>
       </c>
@@ -533,7 +533,7 @@
         <v>0.3953033268101761</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>45738</v>
       </c>
@@ -551,7 +551,7 @@
         <v>0.47619047619047616</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>45752</v>
       </c>
@@ -569,7 +569,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>45752</v>
       </c>
@@ -587,7 +587,7 @@
         <v>0.39506172839506171</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>45773</v>
       </c>
@@ -605,7 +605,7 @@
         <v>-2.3057851239669422</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>45759</v>
       </c>
@@ -623,7 +623,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>45780</v>
       </c>
@@ -641,7 +641,7 @@
         <v>0.31147540983606559</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>45780</v>
       </c>
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>45780</v>
       </c>
@@ -671,7 +671,7 @@
         <v>0.13667820069204153</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>45787</v>
       </c>
@@ -689,7 +689,7 @@
         <v>0.11627906976744186</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>45794</v>
       </c>
@@ -707,19 +707,25 @@
         <v>0.34444444444444444</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>45800</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="C13">
+        <v>171</v>
+      </c>
+      <c r="D13">
+        <v>80</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.53216374269005851</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>45822</v>
       </c>
@@ -731,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>45822</v>
       </c>
@@ -743,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>45836</v>
       </c>
@@ -755,91 +761,91 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="6"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="6"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="6"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="6"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="B34" s="6"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
       <c r="B35" s="7"/>
       <c r="E35" s="1"/>

</xml_diff>

<commit_message>
updated cxs attendance (#1195)
</commit_message>
<xml_diff>
--- a/assets/misc/2025/2025_Attendance.xlsx
+++ b/assets/misc/2025/2025_Attendance.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve.jones\Documents\git\sqlsatwebsite\assets\misc\2025\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B4A342-2BBA-440D-A335-B7E579B9BFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -95,12 +114,21 @@
   </si>
   <si>
     <t>Lost a box of tickets. Not everyone was scanned in. We gave away at least 350 bags.</t>
+  </si>
+  <si>
+    <t>SQL Saturday Boston 2025 (#1119)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Minnesota (#1124)</t>
+  </si>
+  <si>
+    <t>SQL Saturday CXS 2025 (#1125)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
@@ -166,62 +194,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -232,10 +248,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -273,71 +289,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -365,7 +381,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -388,11 +404,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -401,13 +417,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -417,7 +433,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -426,7 +442,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -435,7 +451,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -443,10 +459,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -511,28 +527,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="12" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="50.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="15" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>45724</v>
       </c>
@@ -575,14 +590,11 @@
         <v>309</v>
       </c>
       <c r="E2" s="8">
-        <f>IF(C2=0,0,+(C2-D2)/C2)</f>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+        <f t="shared" ref="E2:E21" si="0">IF(C2=0,0,+(C2-D2)/C2)</f>
+        <v>0.3953033268101761</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>45738</v>
       </c>
@@ -596,14 +608,11 @@
         <v>110</v>
       </c>
       <c r="E3" s="8">
-        <f>IF(C3=0,0,+(C3-D3)/C3)</f>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>45752</v>
       </c>
@@ -617,14 +626,11 @@
         <v>350</v>
       </c>
       <c r="E4" s="8">
-        <f>IF(C4=0,0,+(C4-D4)/C4)</f>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>45752</v>
       </c>
@@ -638,14 +644,11 @@
         <v>98</v>
       </c>
       <c r="E5" s="8">
-        <f>IF(C5=0,0,+(C5-D5)/C5)</f>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0.39506172839506171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>45773</v>
       </c>
@@ -659,14 +662,11 @@
         <v>400</v>
       </c>
       <c r="E6" s="8">
-        <f>IF(C6=0,0,+(C6-D6)/C6)</f>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>-2.3057851239669422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>45759</v>
       </c>
@@ -680,14 +680,11 @@
         <v>69</v>
       </c>
       <c r="E7" s="8">
-        <f>IF(C7=0,0,+(C7-D7)/C7)</f>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>45780</v>
       </c>
@@ -701,31 +698,23 @@
         <v>84</v>
       </c>
       <c r="E8" s="8">
-        <f>IF(C8=0,0,+(C8-D8)/C8)</f>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0.31147540983606559</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>45780</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
       <c r="E9" s="8">
-        <f>IF(C9=0,0,+(C9-D9)/C9)</f>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>45780</v>
       </c>
@@ -739,14 +728,11 @@
         <v>499</v>
       </c>
       <c r="E10" s="8">
-        <f>IF(C10=0,0,+(C10-D10)/C10)</f>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0.13667820069204153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>45787</v>
       </c>
@@ -760,14 +746,11 @@
         <v>190</v>
       </c>
       <c r="E11" s="8">
-        <f>IF(C11=0,0,+(C11-D11)/C11)</f>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0.11627906976744186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>45794</v>
       </c>
@@ -781,14 +764,11 @@
         <v>118</v>
       </c>
       <c r="E12" s="8">
-        <f>IF(C12=0,0,+(C12-D12)/C12)</f>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0.34444444444444444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>45800</v>
       </c>
@@ -802,14 +782,11 @@
         <v>80</v>
       </c>
       <c r="E13" s="8">
-        <f>IF(C13=0,0,+(C13-D13)/C13)</f>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0.53216374269005851</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>45822</v>
       </c>
@@ -823,14 +800,11 @@
         <v>169</v>
       </c>
       <c r="E14" s="8">
-        <f>IF(C14=0,0,+(C14-D14)/C14)</f>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>-1.4142857142857144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>45822</v>
       </c>
@@ -844,254 +818,167 @@
         <v>60</v>
       </c>
       <c r="E15" s="8">
-        <f>IF(C15=0,0,+(C15-D15)/C15)</f>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>45836</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
       <c r="E16" s="8">
-        <f>IF(C16=0,0,+(C16-D16)/C16)</f>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>45857</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
       <c r="E17" s="8">
-        <f>IF(C17=0,0,+(C17-D17)/C17)</f>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>45864</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>611</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>155</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9" t="s">
+      <c r="E18" s="8">
+        <f t="shared" si="0"/>
+        <v>0.74631751227495913</v>
+      </c>
+      <c r="I18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="5"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="11">
+        <v>45927</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19">
+        <v>297</v>
+      </c>
+      <c r="D19">
+        <v>240</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>0.19191919191919191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="11">
+        <v>45927</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="11">
+        <v>45927</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21">
+        <v>187</v>
+      </c>
+      <c r="D21">
+        <v>115</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="0"/>
+        <v>0.38502673796791442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    </row>
+    <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    </row>
+    <row r="24" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    </row>
+    <row r="25" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    </row>
+    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    </row>
+    <row r="27" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    </row>
+    <row r="28" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="15.75">
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="B29" s="10"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    </row>
+    <row r="30" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
+      <c r="B30" s="10"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    </row>
+    <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="10"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    </row>
+    <row r="32" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
+      <c r="B32" s="10"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    </row>
+    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
+      <c r="B33" s="10"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    </row>
+    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
+      <c r="B34" s="10"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    </row>
+    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="B35" s="10"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
st louis and toronto attendance
</commit_message>
<xml_diff>
--- a/assets/misc/2025/2025_Attendance.xlsx
+++ b/assets/misc/2025/2025_Attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve.jones\Documents\git\sqlsatwebsite\assets\misc\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9984876-A2A4-4168-A95E-5A1292D57745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87924CAE-ED4A-44D3-98D0-1D9AF28EFA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>SQL Saturday Orlando 2025 (#1122) </t>
+  </si>
+  <si>
+    <t>SQL Saturday St. Louis 2025 (#1117)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Toronto 2025 (#1131)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Pittsburgh 2025 (#1123) </t>
   </si>
 </sst>
 </file>
@@ -548,20 +557,20 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E22" sqref="A22:E22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>45724</v>
       </c>
@@ -604,11 +613,11 @@
         <v>309</v>
       </c>
       <c r="E2" s="8">
-        <f t="shared" ref="E2:E22" si="0">IF(C2=0,0,+(C2-D2)/C2)</f>
+        <f t="shared" ref="E2:E25" si="0">IF(C2=0,0,+(C2-D2)/C2)</f>
         <v>0.3953033268101761</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>45738</v>
       </c>
@@ -626,7 +635,7 @@
         <v>0.47619047619047616</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>45752</v>
       </c>
@@ -644,7 +653,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>45752</v>
       </c>
@@ -662,7 +671,7 @@
         <v>0.39506172839506171</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>45773</v>
       </c>
@@ -680,7 +689,7 @@
         <v>-2.3057851239669422</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>45759</v>
       </c>
@@ -698,7 +707,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>45780</v>
       </c>
@@ -716,7 +725,7 @@
         <v>0.31147540983606559</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>45780</v>
       </c>
@@ -728,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>45780</v>
       </c>
@@ -746,7 +755,7 @@
         <v>0.13667820069204153</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>45787</v>
       </c>
@@ -764,7 +773,7 @@
         <v>0.11627906976744186</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>45794</v>
       </c>
@@ -782,7 +791,7 @@
         <v>0.34444444444444444</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>45800</v>
       </c>
@@ -800,7 +809,7 @@
         <v>0.53216374269005851</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>45822</v>
       </c>
@@ -818,7 +827,7 @@
         <v>-1.4142857142857144</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>45822</v>
       </c>
@@ -836,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>45836</v>
       </c>
@@ -848,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>45857</v>
       </c>
@@ -860,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>45864</v>
       </c>
@@ -881,7 +890,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>45927</v>
       </c>
@@ -899,7 +908,7 @@
         <v>0.19191919191919191</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>45927</v>
       </c>
@@ -913,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>45927</v>
       </c>
@@ -931,7 +940,7 @@
         <v>0.38502673796791442</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>45934</v>
       </c>
@@ -949,61 +958,97 @@
         <v>0.43820224719101125</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>45948</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>45955</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="9">
+        <v>235</v>
+      </c>
+      <c r="D24" s="9">
+        <v>121</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="0"/>
+        <v>0.48510638297872338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>45955</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="9">
+        <v>367</v>
+      </c>
+      <c r="D25" s="9">
+        <v>289</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="0"/>
+        <v>0.21253405994550409</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="10"/>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="10"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="10"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="10"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="10"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="10"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="10"/>
       <c r="E35" s="8"/>
@@ -1011,7 +1056,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B22" r:id="rId1" display="https://sqlsaturday.com/2025-10-04-sqlsaturday1122/" xr:uid="{6E93A10F-B511-48C1-A833-4D51513D91C4}"/>
+    <hyperlink ref="B24" r:id="rId2" display="https://sqlsaturday.com/2025-10-25-sqlsaturday1117/" xr:uid="{A7DA2FAD-BA1C-4A45-98CC-635263579449}"/>
+    <hyperlink ref="B25" r:id="rId3" display="https://sqlsaturday.com/2025-10-25-sqlsaturday1131/" xr:uid="{F95243ED-E1B2-494F-8F69-B786B43E5557}"/>
+    <hyperlink ref="B23" r:id="rId4" display="https://sqlsaturday.com/2025-10-18-sqlsaturday1123/" xr:uid="{179CE75E-0E5C-41A3-9410-24CEDD56D08D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added test event (#1248)
Co-authored-by: way0utwest <admin@sqlsaturday.com>
</commit_message>
<xml_diff>
--- a/assets/misc/2025/2025_Attendance.xlsx
+++ b/assets/misc/2025/2025_Attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5191146-4A17-45A3-AC6B-2CD92D3066BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B23789-8537-4CE6-9338-DE0EC9D10FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="-300" windowWidth="25935" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4335" yWindow="585" windowWidth="21960" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>SQL Saturday Houston 2025 (#1120)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Lima 2025 (#1126)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Oregon &amp; SW Washington 2025 (#1130)</t>
   </si>
 </sst>
 </file>
@@ -560,7 +566,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E28" sqref="A27:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +622,7 @@
         <v>309</v>
       </c>
       <c r="E2" s="8">
-        <f t="shared" ref="E2:E26" si="0">IF(C2=0,0,+(C2-D2)/C2)</f>
+        <f t="shared" ref="E2:E28" si="0">IF(C2=0,0,+(C2-D2)/C2)</f>
         <v>0.3953033268101761</v>
       </c>
     </row>
@@ -1034,12 +1040,40 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="E27" s="8"/>
+      <c r="A27" s="5">
+        <v>45976</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="9">
+        <v>295</v>
+      </c>
+      <c r="D27" s="9">
+        <v>200</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" si="0"/>
+        <v>0.32203389830508472</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="E28" s="8"/>
+      <c r="A28" s="5">
+        <v>45983</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="9">
+        <v>369</v>
+      </c>
+      <c r="D28" s="9">
+        <v>117</v>
+      </c>
+      <c r="E28" s="8">
+        <f t="shared" si="0"/>
+        <v>0.68292682926829273</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
@@ -1083,8 +1117,10 @@
     <hyperlink ref="B25" r:id="rId3" display="https://sqlsaturday.com/2025-10-25-sqlsaturday1131/" xr:uid="{F95243ED-E1B2-494F-8F69-B786B43E5557}"/>
     <hyperlink ref="B23" r:id="rId4" display="https://sqlsaturday.com/2025-10-18-sqlsaturday1123/" xr:uid="{179CE75E-0E5C-41A3-9410-24CEDD56D08D}"/>
     <hyperlink ref="B26" r:id="rId5" display="https://sqlsaturday.com/2025-11-08-sqlsaturday1120/" xr:uid="{F007E6AC-513D-4E00-9E3B-C68947357F5F}"/>
+    <hyperlink ref="B28" r:id="rId6" display="https://sqlsaturday.com/2025-11-22-sqlsaturday1126/" xr:uid="{CDDA5F51-FCDF-41A5-81CE-3A70B20F7D25}"/>
+    <hyperlink ref="B27" r:id="rId7" display="https://sqlsaturday.com/2025-11-15-sqlsaturday1130/" xr:uid="{A8D7C901-AD32-4918-88DB-18074CD12BC1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>